<commit_message>
Added additional log messages to db
</commit_message>
<xml_diff>
--- a/log_messages.xlsx
+++ b/log_messages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hbreaux\Documents\Programs\Test Programs\Log Parser for CP Support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57875CA-9068-4C67-97DB-94B753B5ED30}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259145B5-9340-4007-AFA9-E6D056E9CBF6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11325" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -148,7 +148,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="44">
   <si>
     <t>This database is meant to serve as a repository of common log messages and their meanings.  Log messages must always be interpreted in the context of what is around them.  This database is not meant to be a replacement for troubleshooting and it is not intended to interpret logs for you.  This repository has been designed as an assistant to help engineers work with logs more effeciently.  Anyone using it must be careful not to let it act as a replacement for their own critical thinking and reasoning skills. </t>
   </si>
@@ -186,9 +186,6 @@
     <t>WAN</t>
   </si>
   <si>
-    <t>WAN:.*| signal MC400LP6 (SIM1) on port modem1: .*%, RSSI:-.*(dBm), SINR:.*(dB), RSRP:-.*(dB), RSRQ:-.*(dB), RFBAND: Band .*</t>
-  </si>
-  <si>
     <t>These message appear peridoically in the log of a Cradlepoint with a modem.  The values in them indicate the signal strength of the modem.  Look at the timestamp to determine what time the signal strength information is from.  If youre running into intermittent connectivity issues, check these message to see if you have poor signal strength.  See this article for help interpretting whether your signal strength values are good or poor: https://customer.cradlepoint.com/s/article/Modem-Signal-Strength-and-Signal-Quality</t>
   </si>
   <si>
@@ -247,6 +244,42 @@
   </si>
   <si>
     <t>This message appears after a device has succesfully connected to Netcloud</t>
+  </si>
+  <si>
+    <t>Problematic</t>
+  </si>
+  <si>
+    <t>WAN:.*|SIM error: NOSIM</t>
+  </si>
+  <si>
+    <t>WARN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The SIM card is not inserted, it is inserted improperly, either the SIM or the port for the SIM may be bad, or you have an incorrect size of SIM card. If the SIM is inserted properly, and is the correct size, and you are still getting the NO SIM error, then you need to test the SIM card in a different device to eliminate the SIM being the issue. https://customer.cradlepoint.com/s/article/What-type-of-SIM-cards-do-CradlePoint-modems-use </t>
+  </si>
+  <si>
+    <t>suspending due to IP conflict </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Cradlepoint is detecting an IP Conflict, usually this happens when there is something on the network that has the same IP address as the one of the Cradlepoint's networks.  The most common appearance of this is when the WAN connection is trying to use an IP Address that is within the same IP address of one of the Cradlepoint's LANs.  To resolve that, change the subnet of your LAN, or get the WAN to give out addresses on a non-conflicting range. </t>
+  </si>
+  <si>
+    <t>Connect Event: unknown error - state: connecting</t>
+  </si>
+  <si>
+    <t>state=connecting result=unknown error</t>
+  </si>
+  <si>
+    <t>WAN:.*| signal .* (S.*) on port modem1: .*%, RSSI:-.*(dBm), SINR:.*(dB), RSRP:-.*(dB), RSRQ:-.*(dB), RFBAND: Band .*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A CPPM unknown error usually indicates the modem or SIM is not functioning properly.  It can also indicate modem/SIM card provisioning errors.  </t>
+  </si>
+  <si>
+    <t>Module FW(.*) / SIM Carrier(.*) - mismatch</t>
+  </si>
+  <si>
+    <t>Indicates a mismatch between the modem firmware and the SIM. It is most likely to occur on modems that do not support Auto Carrier Selection. For modems that do not support Auto-Carrier Selection, ensure the correct firmware is loaded. For information about modem firmware management, click https://customer.cradlepoint.com/s/article/NCOS-Cradlepoint-Manual-Modem-Firmware-Update.</t>
   </si>
 </sst>
 </file>
@@ -337,7 +370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -373,6 +406,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -801,11 +840,11 @@
   <sheetPr>
     <tabColor rgb="FFFCE4D6"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,7 +856,7 @@
     <col min="5" max="6" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
@@ -830,8 +869,11 @@
       <c r="D1" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="E1" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -839,27 +881,33 @@
         <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E3" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -867,13 +915,16 @@
         <v>11</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E4" s="15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -881,27 +932,33 @@
         <v>11</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="E5" s="15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E6" s="15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -909,13 +966,16 @@
         <v>11</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E7" s="15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -923,28 +983,120 @@
         <v>11</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="E8" s="15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>27</v>
+      <c r="E9" s="15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="15" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1087,13 +1239,13 @@
         <v>10</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1101,13 +1253,13 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
         <v>31</v>
-      </c>
-      <c r="D3" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>